<commit_message>
Pillow config added. New pillow excel added. Pillow entry changed for new product.
</commit_message>
<xml_diff>
--- a/ChairishRugEntry/2389-2450.xlsx
+++ b/ChairishRugEntry/2389-2450.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\okkaa\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasan\PycharmProjects\wovenyChairishPillowEntry\ChairishRugEntry\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2282,7 +2282,7 @@
   <dimension ref="A1:Z160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2826,7 +2826,7 @@
         <v>1</v>
       </c>
       <c r="D9" s="2">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E9" s="2">
         <v>290</v>

</xml_diff>